<commit_message>
chore: update variable name
Replace variable name in file transitory_input.xlsx as follows:

    * MLT_UPPER -> MLT_INCREASE
    * MLT_LOWER -> MLT_DECREASE

modified:   input_files/input_file_template/template_transitory_input.xlsx
modified:   simulation_global_info.py
modified:   utility_functions/transient_solution_functions.py
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_transitory_input.xlsx
+++ b/source_code/input_files/input_file_template/template_transitory_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839D6F6-D5C9-4831-8E81-79B91603EFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0CD5F4-0481-4F6E-962A-CB49A14B3D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,12 +119,6 @@
     <t>template_environment_input.xlsx</t>
   </si>
   <si>
-    <t>MLT_UPPER</t>
-  </si>
-  <si>
-    <t>MLT_LOWER</t>
-  </si>
-  <si>
     <t>float or str</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>End time of the simulation</t>
+  </si>
+  <si>
+    <t>MLT_INCREASE</t>
+  </si>
+  <si>
+    <t>MLT_DECREASE</t>
   </si>
 </sst>
 </file>
@@ -262,7 +262,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="GRID"/>
@@ -583,10 +583,10 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2">
         <v>100</v>
@@ -703,9 +703,9 @@
         <v>11</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2">
+        <v>30</v>
+      </c>
+      <c r="E7" s="10">
         <v>0</v>
       </c>
     </row>
@@ -720,9 +720,9 @@
         <v>10</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2">
+        <v>31</v>
+      </c>
+      <c r="E8" s="10">
         <v>0.1</v>
       </c>
     </row>
@@ -737,38 +737,44 @@
         <v>10</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2">
+        <v>32</v>
+      </c>
+      <c r="E9" s="10">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>31</v>
+      <c r="E11" s="10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -784,7 +790,7 @@
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="10">
         <v>100</v>
       </c>
     </row>
@@ -801,7 +807,7 @@
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="10">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore!: new variable TIME_STEP in file template_transitory_input.xlsx
Added new variable to specify the value of the time step for the thermal-hydraulic loop in file template_transitory_input.xlsx.
If flag IADAPTIME = 0, TIME_STEP value is used as uniform time step for the thermal-hydraulic loop; if flag IADAPTIME = 1 or 2, TIME_STEP value may be tuned according to the adaptive time step criterion.

BREAKING CHANGES: the add variable in input file template_transitory_input.xlsx could make it not compatible with older version of the code.

modified:   input_files/input_file_template/template_transitory_input.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_transitory_input.xlsx
+++ b/source_code/input_files/input_file_template/template_transitory_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0CD5F4-0481-4F6E-962A-CB49A14B3D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE840C90-FB71-457E-8810-3FEA78A0FA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>SIMULATION</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>MLT_DECREASE</t>
+  </si>
+  <si>
+    <t>TIME_STEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User defined time step for the thermal-hydraulic loop. Should be in the range [STPMIN, STPMAX] (boundary included). </t>
   </si>
 </sst>
 </file>
@@ -580,13 +586,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,A6,E6,A8,E8,[1]GRID!$A$4,[1]GRID!$E$4,"template")</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,A6,E6,A9,E9,[1]GRID!$A$4,[1]GRID!$E$4,"template")</f>
         <v>TEND_100_STPMIN_0.1_NELEMS_200_template</v>
       </c>
     </row>
@@ -711,7 +717,7 @@
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>2</v>
@@ -720,15 +726,15 @@
         <v>10</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E8" s="10">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>2</v>
@@ -737,32 +743,32 @@
         <v>10</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="10">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" s="10">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>12</v>
@@ -770,33 +776,33 @@
       <c r="C11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E12" s="10">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="10">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
@@ -805,9 +811,26 @@
         <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E14" s="10">
         <v>5</v>
       </c>
     </row>

</xml_diff>